<commit_message>
Tu mensaje de commit aquí
</commit_message>
<xml_diff>
--- a/actitud.xlsx
+++ b/actitud.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef4cc4ddfd4d7cd1/Github/3C/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_F25DC773A252ABDACC10482D291E55885BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8CE2F47-72D7-4EFC-B8CF-7B37487A235E}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABDACC10482D291E55885BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB784CFB-AF48-43E7-85C4-B93C4A91C66E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Astronauta" sheetId="1" r:id="rId1"/>
@@ -245,6 +245,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,17 +516,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L27" sqref="L27:L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -569,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -578,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -587,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -596,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -605,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -614,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -623,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -632,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -641,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -650,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -659,7 +663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -668,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -677,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -686,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -695,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -704,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -713,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -722,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -731,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -740,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -749,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -758,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -767,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -776,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -785,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -794,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -817,12 +821,12 @@
       <selection activeCell="L27" sqref="L27:L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -860,7 +864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -869,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -878,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -887,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -896,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -905,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -914,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -923,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -932,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -941,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -950,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -959,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -968,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -977,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -986,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -995,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1013,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1031,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1049,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1058,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1067,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1076,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1085,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1116,12 +1120,12 @@
       <selection activeCell="L27" sqref="L27:L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1168,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1177,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1186,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1204,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1213,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1222,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1231,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1240,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1267,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1276,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1285,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1312,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1321,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1330,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1348,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1357,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1366,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1375,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1384,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1393,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1411,16 +1415,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45A07B9-F651-41BC-A481-395AA628394B}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27:P28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1470,247 +1474,328 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="P2">
         <f>IFERROR(SUM(B2:O2)/COUNT(B2:O2)*100, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="P3">
         <f t="shared" ref="P3:P28" si="0">IFERROR(SUM(B3:O3)/COUNT(B3:O3)*100, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="P10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
       <c r="P11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
       <c r="P12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="P14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
       <c r="P15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
       <c r="P16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="P17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
       <c r="P18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
       <c r="P19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
       <c r="P20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
       <c r="P21">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
       <c r="P22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
       <c r="P23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
       <c r="P24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
       <c r="P25">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
       <c r="P26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
       <c r="P27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
       <c r="P28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>